<commit_message>
Add function to resume transactions in month
</commit_message>
<xml_diff>
--- a/Saida.xlsx
+++ b/Saida.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2e8a693e5135478/Projetos JS/ceiScraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{CA3825A4-9028-46C5-A877-F79050E3D2B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0C5C2CDD-32B9-4D15-84FE-E1B590990457}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{CA3825A4-9028-46C5-A877-F79050E3D2B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC8C578D-CB26-455D-A2DB-76061528BEAE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3836B8AC-7ABC-4B5D-B557-3A34897B32B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
   <si>
     <t>CNPJ</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>XXX</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
 </sst>
 </file>
@@ -85,12 +88,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,14 +122,24 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -431,15 +456,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B283B24B-06B0-42DE-8680-DE1DE03DF161}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -455,8 +485,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -466,11 +499,184 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
-        <v>15.5</v>
+      <c r="E2" s="2">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43860</v>
+      </c>
+      <c r="H2" s="8">
+        <f>E2*D2</f>
+        <v>160</v>
+      </c>
+      <c r="I2">
+        <f>16</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43860</v>
+      </c>
+      <c r="H4" s="8">
+        <f>E4*D4</f>
+        <v>15</v>
+      </c>
+      <c r="I4" s="8">
+        <f>(H2+H4)/(D2+D4)</f>
+        <v>15.909090909090908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43860</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:H7" si="0">E5*D5</f>
+        <v>28</v>
+      </c>
+      <c r="I5" s="8">
+        <f>((I4*11)+(D5*E5))/(11+2)</f>
+        <v>15.615384615384615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43860</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="0"/>
+        <v>-26</v>
+      </c>
+      <c r="I6" s="8">
+        <f>((I4*11)+(D5*E5))/(11+2)</f>
+        <v>15.615384615384615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <v>43860</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3">
+        <v>43889</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="1">
+        <v>-10</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="3">
+        <v>43889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>